<commit_message>
exemplars_similarity task ready to be Compiled in Pavlovia
</commit_message>
<xml_diff>
--- a/exemplars_similarity/design.xlsx
+++ b/exemplars_similarity/design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/santiago_castiellodeobeso_yale_edu/Documents/Collaborations/Brooklyn_College/categoricalReversalLerning/exemplars_similarity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="11_F25DC773A252ABDACC10482A911958D25BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{525CDC12-7650-4678-BA85-23F4A78D60BB}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="11_F25DC773A252ABDACC10482A911958D25BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C293E51-D0C4-4544-BA24-486194F80A2F}"/>
   <bookViews>
-    <workbookView xWindow="66195" yWindow="5850" windowWidth="18900" windowHeight="9825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="design" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="25">
   <si>
     <t>Task 1</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Task  2</t>
+  </si>
+  <si>
+    <t>Task 2</t>
   </si>
 </sst>
 </file>
@@ -471,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:U11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -495,7 +498,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="L1" s="4" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
@@ -1033,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9BA94A-73EE-407E-9CB2-EE0A23D577E8}">
   <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I42" workbookViewId="0">
-      <selection activeCell="V42" sqref="V1:V1048576"/>
+    <sheetView topLeftCell="G1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>

</xml_diff>

<commit_message>
MDS matrices sent to Andy
</commit_message>
<xml_diff>
--- a/exemplars_similarity/design.xlsx
+++ b/exemplars_similarity/design.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="155" documentId="11_F25DC773A252ABDACC10482A911958D25BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C293E51-D0C4-4544-BA24-486194F80A2F}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="design" sheetId="1" r:id="rId1"/>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N4" sqref="N4:U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -1036,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9BA94A-73EE-407E-9CB2-EE0A23D577E8}">
   <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:U1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>

</xml_diff>

<commit_message>
manuscript v3 sent to andy
</commit_message>
<xml_diff>
--- a/exemplars_similarity/design.xlsx
+++ b/exemplars_similarity/design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/santiago_castiellodeobeso_yale_edu/Documents/Collaborations/Brooklyn_College/categoricalReversalLerning/exemplars_similarity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/santiago_castiellodeobeso_yale_edu/Documents/Collaborations/Brooklyn_College/representingCategories/categoricalReversalLerning/exemplars_similarity/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="155" documentId="11_F25DC773A252ABDACC10482A911958D25BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C293E51-D0C4-4544-BA24-486194F80A2F}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="design" sheetId="1" r:id="rId1"/>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:U11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -1036,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9BA94A-73EE-407E-9CB2-EE0A23D577E8}">
   <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="G2" zoomScale="138" workbookViewId="0">
+      <selection activeCell="M57" sqref="M2:N57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>

</xml_diff>